<commit_message>
Updated to 1/24/2020 for Wuhan nCoV dataset
</commit_message>
<xml_diff>
--- a/wuhan_nCoV_2020.xlsx
+++ b/wuhan_nCoV_2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19035" windowHeight="11055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19035" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="数据" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>新增病例</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,6 +107,10 @@
   </si>
   <si>
     <t>1月7日-11日，武汉“两会”；1月8日-18日，湖北省“二会”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>武汉市宣部封城</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -169,7 +173,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -179,6 +183,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -462,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -573,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J16" si="1">G5-H5-I5</f>
+        <f t="shared" ref="J5:J15" si="1">G5-H5-I5</f>
         <v>33</v>
       </c>
       <c r="K5">
@@ -1029,16 +1034,76 @@
       <c r="B16" s="1">
         <v>43853</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C16">
+        <v>70</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>495</v>
+      </c>
+      <c r="H16">
+        <v>23</v>
+      </c>
+      <c r="I16">
+        <v>31</v>
+      </c>
+      <c r="J16">
+        <v>441</v>
+      </c>
+      <c r="K16">
+        <v>61</v>
+      </c>
+      <c r="L16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17" s="1">
         <v>43854</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C17">
+        <v>77</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>572</v>
+      </c>
+      <c r="H17">
+        <v>38</v>
+      </c>
+      <c r="I17">
+        <v>32</v>
+      </c>
+      <c r="J17">
+        <v>502</v>
+      </c>
+      <c r="K17">
+        <v>61</v>
+      </c>
+      <c r="L17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1046,7 +1111,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1054,7 +1119,7 @@
         <v>43856</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1062,7 +1127,7 @@
         <v>43857</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1070,7 +1135,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1078,7 +1143,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1086,7 +1151,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1094,7 +1159,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1102,7 +1167,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1110,32 +1175,32 @@
         <v>43863</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1163,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1184,57 +1249,65 @@
       <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
+      <c r="A3" s="5">
+        <v>43853</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="4">
-        <v>43849</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
-        <v>43841</v>
+        <v>43849</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
-        <v>43835</v>
+        <v>43841</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
-        <v>43833</v>
+        <v>43835</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
+        <v>43833</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="4">
         <v>44196</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to 1/24/2020 for Wuhan nCov
</commit_message>
<xml_diff>
--- a/wuhan_nCoV_2020.xlsx
+++ b/wuhan_nCoV_2020.xlsx
@@ -39,10 +39,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dR/dt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>累计病例</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -111,6 +107,10 @@
   </si>
   <si>
     <t>武汉市宣部封城</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dR/dt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -465,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -476,7 +476,7 @@
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -486,39 +486,39 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>0</v>
       </c>
@@ -547,8 +547,12 @@
         <f>G4-H4-I4</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M4">
+        <f>(H5+I5)-(H4-I4)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -564,10 +568,6 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F15" si="0">(D5+E5)-(D4+E4)</f>
-        <v>-3</v>
-      </c>
       <c r="G5">
         <v>41</v>
       </c>
@@ -578,19 +578,23 @@
         <v>7</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J15" si="1">G5-H5-I5</f>
+        <f t="shared" ref="J5:J15" si="0">G5-H5-I5</f>
         <v>33</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K15" si="2">J5-J4</f>
+        <f t="shared" ref="K5:K15" si="1">J5-J4</f>
         <v>-1</v>
       </c>
       <c r="L5">
         <f>C5-K5</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M5">
+        <f t="shared" ref="M5:M17" si="2">(H6+I6)-(H5-I5)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2</v>
       </c>
@@ -606,10 +610,6 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
       <c r="G6">
         <v>41</v>
       </c>
@@ -620,19 +620,23 @@
         <v>7</v>
       </c>
       <c r="J6">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L6">
         <f t="shared" ref="L6:L15" si="3">C6-K6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>3</v>
       </c>
@@ -648,10 +652,6 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="G7">
         <v>41</v>
       </c>
@@ -662,19 +662,23 @@
         <v>7</v>
       </c>
       <c r="J7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>4</v>
       </c>
@@ -690,10 +694,6 @@
       <c r="E8">
         <v>5</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
       <c r="G8">
         <v>41</v>
       </c>
@@ -704,19 +704,23 @@
         <v>12</v>
       </c>
       <c r="J8">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>5</v>
       </c>
@@ -731,10 +735,6 @@
       </c>
       <c r="E9">
         <v>3</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>-3</v>
       </c>
       <c r="G9">
         <f>C9+G8</f>
@@ -749,19 +749,23 @@
         <v>15</v>
       </c>
       <c r="J9">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>6</v>
       </c>
@@ -776,10 +780,6 @@
       </c>
       <c r="E10">
         <v>4</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:I15" si="4">C10+G9</f>
@@ -794,19 +794,23 @@
         <v>19</v>
       </c>
       <c r="J10">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="L10">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>7</v>
       </c>
@@ -821,10 +825,6 @@
       </c>
       <c r="E11">
         <v>5</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>2</v>
       </c>
       <c r="G11">
         <f t="shared" si="4"/>
@@ -839,19 +839,23 @@
         <v>24</v>
       </c>
       <c r="J11">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>8</v>
       </c>
@@ -866,10 +870,6 @@
       </c>
       <c r="E12">
         <v>0</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>-5</v>
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
@@ -882,19 +882,23 @@
         <v>24</v>
       </c>
       <c r="J12">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>9</v>
       </c>
@@ -909,10 +913,6 @@
       </c>
       <c r="E13">
         <v>0</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="G13">
         <f t="shared" si="4"/>
@@ -925,19 +925,23 @@
         <v>25</v>
       </c>
       <c r="J13">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="1"/>
-        <v>227</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="L13">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>10</v>
       </c>
@@ -952,10 +956,6 @@
       </c>
       <c r="E14">
         <v>3</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>4</v>
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
@@ -970,19 +970,23 @@
         <v>28</v>
       </c>
       <c r="J14">
+        <f t="shared" si="0"/>
+        <v>326</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="1"/>
-        <v>326</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="L14">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>11</v>
       </c>
@@ -997,10 +1001,6 @@
       </c>
       <c r="E15">
         <v>0</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>2</v>
       </c>
       <c r="G15">
         <f t="shared" si="4"/>
@@ -1015,19 +1015,23 @@
         <v>28</v>
       </c>
       <c r="J15">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="1"/>
-        <v>380</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="L15">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1043,9 +1047,6 @@
       <c r="E16">
         <v>3</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
       <c r="G16">
         <v>495</v>
       </c>
@@ -1064,8 +1065,12 @@
       <c r="L16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1081,9 +1086,6 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17">
-        <v>7</v>
-      </c>
       <c r="G17">
         <v>572</v>
       </c>
@@ -1102,8 +1104,12 @@
       <c r="L17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1111,7 +1117,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1119,7 +1125,7 @@
         <v>43856</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1127,7 +1133,7 @@
         <v>43857</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1135,7 +1141,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1143,7 +1149,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1151,7 +1157,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1175,32 +1181,32 @@
         <v>43863</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1242,7 +1248,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -1253,17 +1259,17 @@
         <v>43853</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
@@ -1271,7 +1277,7 @@
         <v>43849</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
@@ -1279,7 +1285,7 @@
         <v>43841</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
@@ -1287,7 +1293,7 @@
         <v>43835</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
@@ -1295,7 +1301,7 @@
         <v>43833</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
@@ -1303,12 +1309,12 @@
         <v>44196</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to 1/25/2020 for Wuhan nCoV
</commit_message>
<xml_diff>
--- a/wuhan_nCoV_2020.xlsx
+++ b/wuhan_nCoV_2020.xlsx
@@ -106,11 +106,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>武汉市宣部封城</t>
+    <t>dR/dt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dR/dt</t>
+    <t>武汉市宣部从早10点开始封城</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -173,7 +173,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -184,6 +184,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,7 +471,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -505,7 +508,7 @@
         <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
@@ -547,10 +550,6 @@
         <f>G4-H4-I4</f>
         <v>34</v>
       </c>
-      <c r="M4">
-        <f>(H5+I5)-(H4-I4)</f>
-        <v>13</v>
-      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5">
@@ -590,8 +589,8 @@
         <v>1</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M17" si="2">(H6+I6)-(H5-I5)</f>
-        <v>14</v>
+        <f>(H5+I5)-(H4+I4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
@@ -628,12 +627,12 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <f t="shared" ref="L6:L15" si="3">C6-K6</f>
+        <f t="shared" ref="L6:L15" si="2">C6-K6</f>
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="2"/>
-        <v>14</v>
+        <f t="shared" ref="M6:M18" si="3">(H6+I6)-(H5+I5)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
@@ -670,12 +669,12 @@
         <v>0</v>
       </c>
       <c r="L7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="3"/>
         <v>0</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="2"/>
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
@@ -712,12 +711,12 @@
         <v>-6</v>
       </c>
       <c r="L8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="3"/>
         <v>6</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="2"/>
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
@@ -757,12 +756,12 @@
         <v>1</v>
       </c>
       <c r="L9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="3"/>
         <v>3</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
@@ -802,12 +801,12 @@
         <v>13</v>
       </c>
       <c r="L10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="3"/>
         <v>4</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="2"/>
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.15">
@@ -847,12 +846,12 @@
         <v>53</v>
       </c>
       <c r="L11">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="3"/>
         <v>6</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
@@ -890,12 +889,12 @@
         <v>76</v>
       </c>
       <c r="L12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="3"/>
         <v>1</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
@@ -933,12 +932,12 @@
         <v>57</v>
       </c>
       <c r="L13">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="3"/>
         <v>3</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="2"/>
-        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
@@ -978,12 +977,12 @@
         <v>99</v>
       </c>
       <c r="L14">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="3"/>
         <v>6</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
-        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
@@ -1023,12 +1022,12 @@
         <v>54</v>
       </c>
       <c r="L15">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="3"/>
         <v>8</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
@@ -1066,8 +1065,8 @@
         <v>9</v>
       </c>
       <c r="M16">
-        <f t="shared" si="2"/>
-        <v>78</v>
+        <f t="shared" si="3"/>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
@@ -1105,8 +1104,8 @@
         <v>16</v>
       </c>
       <c r="M17">
-        <f t="shared" si="2"/>
-        <v>-6</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
@@ -1115,6 +1114,43 @@
       </c>
       <c r="B18" s="1">
         <v>43855</v>
+      </c>
+      <c r="C18">
+        <v>46</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <f>G17+C18</f>
+        <v>618</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:I18" si="5">H17+D18</f>
+        <v>45</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" ref="J18" si="6">G18-H18-I18</f>
+        <v>533</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ref="K18" si="7">J18-J17</f>
+        <v>31</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18" si="8">C18-K18</f>
+        <v>15</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
@@ -1237,7 +1273,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1259,7 +1295,7 @@
         <v>43853</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Updated to 1/29/2020 for Wuhan nCoV
added data for Hubei province and the whole country
</commit_message>
<xml_diff>
--- a/wuhan_nCoV_2020.xlsx
+++ b/wuhan_nCoV_2020.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19035" windowHeight="11055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19035" windowHeight="11055" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="数据" sheetId="1" r:id="rId1"/>
-    <sheet name="说明" sheetId="2" r:id="rId2"/>
+    <sheet name="wuhan" sheetId="1" r:id="rId1"/>
+    <sheet name="hubei" sheetId="3" r:id="rId2"/>
+    <sheet name="china" sheetId="4" r:id="rId3"/>
+    <sheet name="说明" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>新增病例</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +97,53 @@
   </si>
   <si>
     <t>武汉市宣部从早10点开始封城</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增病例</t>
+  </si>
+  <si>
+    <t>死亡</t>
+  </si>
+  <si>
+    <t>治愈</t>
+  </si>
+  <si>
+    <t>医护</t>
+  </si>
+  <si>
+    <t>累计病例</t>
+  </si>
+  <si>
+    <t>累计死亡</t>
+  </si>
+  <si>
+    <t>累计治愈</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>共接诊</t>
+  </si>
+  <si>
+    <t>留观</t>
+  </si>
+  <si>
+    <t>数据来自湖北卫健委通告： http://wjw.hubei.gov.cn/bmdt/ztzl/fkxxgzbdgrfyyq/xxfb/</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>数据来自国家卫健委通告： http://www.nhc.gov.cn/xcs/yqfkdt/gzbd_index.shtml, 最早连续发布日期委1/21/2020， 发布1/20/2020的疫情通告</t>
+  </si>
+  <si>
+    <t>发热门诊接诊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>留观</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -102,6 +151,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +209,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -168,7 +220,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -452,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -463,7 +518,7 @@
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -482,18 +537,24 @@
       <c r="I1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>0</v>
       </c>
@@ -519,7 +580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -545,7 +606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2</v>
       </c>
@@ -571,7 +632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>3</v>
       </c>
@@ -597,7 +658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>4</v>
       </c>
@@ -623,7 +684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>5</v>
       </c>
@@ -652,7 +713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>6</v>
       </c>
@@ -681,7 +742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>7</v>
       </c>
@@ -710,7 +771,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>8</v>
       </c>
@@ -737,7 +798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>9</v>
       </c>
@@ -764,7 +825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>10</v>
       </c>
@@ -793,7 +854,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>11</v>
       </c>
@@ -822,7 +883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>12</v>
       </c>
@@ -848,7 +909,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>13</v>
       </c>
@@ -874,7 +935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>14</v>
       </c>
@@ -902,41 +963,142 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19" s="1">
         <v>43856</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C19">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <f>G18+C19</f>
+        <v>698</v>
+      </c>
+      <c r="H19">
+        <f>H18+D19</f>
+        <v>63</v>
+      </c>
+      <c r="I19">
+        <f>I18+E19</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" s="1">
         <v>43857</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C20">
+        <v>892</v>
+      </c>
+      <c r="D20">
+        <v>22</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>G19+C20</f>
+        <v>1590</v>
+      </c>
+      <c r="H20">
+        <f>H19+D20</f>
+        <v>85</v>
+      </c>
+      <c r="I20" s="7">
+        <f>I19+E20</f>
+        <v>42</v>
+      </c>
+      <c r="J20">
+        <v>10261</v>
+      </c>
+      <c r="K20">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="B21" s="1">
         <v>43858</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C21">
+        <v>315</v>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>G20+C21</f>
+        <v>1905</v>
+      </c>
+      <c r="H21">
+        <f>H20+D21</f>
+        <v>104</v>
+      </c>
+      <c r="I21" s="7">
+        <f>I20+E21</f>
+        <v>42</v>
+      </c>
+      <c r="J21">
+        <v>10702</v>
+      </c>
+      <c r="K21">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>18</v>
       </c>
       <c r="B22" s="1">
         <v>43859</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C22">
+        <v>356</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <f>G21+C22</f>
+        <v>2261</v>
+      </c>
+      <c r="H22">
+        <f>H21+D22</f>
+        <v>129</v>
+      </c>
+      <c r="I22">
+        <f>I21+E22</f>
+        <v>49</v>
+      </c>
+      <c r="J22">
+        <v>12263</v>
+      </c>
+      <c r="K22">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>19</v>
       </c>
@@ -944,7 +1106,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>20</v>
       </c>
@@ -952,7 +1114,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>21</v>
       </c>
@@ -960,7 +1122,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>22</v>
       </c>
@@ -968,32 +1130,32 @@
         <v>43863</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1020,6 +1182,848 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43842</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43843</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43844</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43846</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43847</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43848</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43849</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43850</v>
+      </c>
+      <c r="C13">
+        <v>72</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>270</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>25</v>
+      </c>
+      <c r="J13">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43851</v>
+      </c>
+      <c r="C14">
+        <v>105</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>375</v>
+      </c>
+      <c r="H14">
+        <v>9</v>
+      </c>
+      <c r="I14">
+        <v>28</v>
+      </c>
+      <c r="J14">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1">
+        <v>43852</v>
+      </c>
+      <c r="C15">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>444</v>
+      </c>
+      <c r="H15">
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>28</v>
+      </c>
+      <c r="J15">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43853</v>
+      </c>
+      <c r="C16">
+        <v>105</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>549</v>
+      </c>
+      <c r="H16">
+        <v>24</v>
+      </c>
+      <c r="I16">
+        <v>31</v>
+      </c>
+      <c r="J16">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1">
+        <v>43854</v>
+      </c>
+      <c r="C17">
+        <v>180</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>729</v>
+      </c>
+      <c r="H17">
+        <v>39</v>
+      </c>
+      <c r="I17">
+        <v>32</v>
+      </c>
+      <c r="J17">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>43855</v>
+      </c>
+      <c r="C18">
+        <v>323</v>
+      </c>
+      <c r="D18">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>1052</v>
+      </c>
+      <c r="H18">
+        <v>52</v>
+      </c>
+      <c r="I18">
+        <v>42</v>
+      </c>
+      <c r="J18">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>43856</v>
+      </c>
+      <c r="C19">
+        <v>371</v>
+      </c>
+      <c r="D19">
+        <v>24</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>1423</v>
+      </c>
+      <c r="H19">
+        <v>76</v>
+      </c>
+      <c r="I19">
+        <v>44</v>
+      </c>
+      <c r="J19">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43857</v>
+      </c>
+      <c r="C20">
+        <v>1291</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>2714</v>
+      </c>
+      <c r="H20">
+        <v>100</v>
+      </c>
+      <c r="I20">
+        <v>47</v>
+      </c>
+      <c r="J20">
+        <v>2567</v>
+      </c>
+      <c r="K20">
+        <v>31934</v>
+      </c>
+      <c r="L20">
+        <v>3759</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43858</v>
+      </c>
+      <c r="C21">
+        <v>840</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <v>33</v>
+      </c>
+      <c r="G21">
+        <v>3554</v>
+      </c>
+      <c r="H21">
+        <v>125</v>
+      </c>
+      <c r="I21">
+        <v>80</v>
+      </c>
+      <c r="J21">
+        <v>3349</v>
+      </c>
+      <c r="K21">
+        <v>31639</v>
+      </c>
+      <c r="L21">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1">
+        <v>43859</v>
+      </c>
+      <c r="C22">
+        <v>1032</v>
+      </c>
+      <c r="D22">
+        <v>37</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>4586</v>
+      </c>
+      <c r="H22">
+        <v>162</v>
+      </c>
+      <c r="I22">
+        <v>90</v>
+      </c>
+      <c r="J22">
+        <v>4334</v>
+      </c>
+      <c r="K22">
+        <v>32309</v>
+      </c>
+      <c r="L22">
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" s="1">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1">
+        <v>43863</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B4" s="6">
+        <v>43841</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B5" s="6">
+        <v>43842</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B6" s="6">
+        <v>43843</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B7" s="6">
+        <v>43844</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B8" s="6">
+        <v>43845</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B9" s="6">
+        <v>43846</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B10" s="6">
+        <v>43847</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B11" s="6">
+        <v>43848</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B12" s="6">
+        <v>43849</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B13" s="6">
+        <v>43850</v>
+      </c>
+      <c r="C13">
+        <v>77</v>
+      </c>
+      <c r="G13">
+        <v>291</v>
+      </c>
+      <c r="L13">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B14" s="6">
+        <v>43851</v>
+      </c>
+      <c r="C14">
+        <v>149</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>440</v>
+      </c>
+      <c r="H14">
+        <v>9</v>
+      </c>
+      <c r="I14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B15" s="6">
+        <v>43852</v>
+      </c>
+      <c r="C15">
+        <v>131</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>571</v>
+      </c>
+      <c r="H15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B16" s="6">
+        <v>43853</v>
+      </c>
+      <c r="C16">
+        <v>259</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>830</v>
+      </c>
+      <c r="H16">
+        <v>25</v>
+      </c>
+      <c r="I16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B17" s="6">
+        <v>43854</v>
+      </c>
+      <c r="C17">
+        <v>444</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>1287</v>
+      </c>
+      <c r="H17">
+        <v>41</v>
+      </c>
+      <c r="I17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B18" s="6">
+        <v>43855</v>
+      </c>
+      <c r="C18">
+        <v>688</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="G18">
+        <v>1975</v>
+      </c>
+      <c r="H18">
+        <v>56</v>
+      </c>
+      <c r="I18">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B19" s="6">
+        <v>43856</v>
+      </c>
+      <c r="C19">
+        <v>769</v>
+      </c>
+      <c r="D19">
+        <v>24</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>2744</v>
+      </c>
+      <c r="H19">
+        <v>80</v>
+      </c>
+      <c r="I19">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B20" s="6">
+        <v>43857</v>
+      </c>
+      <c r="C20">
+        <v>1771</v>
+      </c>
+      <c r="D20">
+        <v>26</v>
+      </c>
+      <c r="E20">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>4515</v>
+      </c>
+      <c r="H20">
+        <v>106</v>
+      </c>
+      <c r="I20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B21" s="6">
+        <v>43858</v>
+      </c>
+      <c r="C21">
+        <v>1459</v>
+      </c>
+      <c r="D21">
+        <v>26</v>
+      </c>
+      <c r="E21">
+        <v>43</v>
+      </c>
+      <c r="G21">
+        <v>5974</v>
+      </c>
+      <c r="H21">
+        <v>132</v>
+      </c>
+      <c r="I21">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B22" s="6">
+        <v>43859</v>
+      </c>
+      <c r="C22">
+        <v>1737</v>
+      </c>
+      <c r="D22">
+        <v>38</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="G22">
+        <v>7711</v>
+      </c>
+      <c r="H22">
+        <v>170</v>
+      </c>
+      <c r="I22">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B23" s="6">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B24" s="6">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B25" s="6">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B26" s="6">
+        <v>43863</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>

</xml_diff>